<commit_message>
new results. 2021/05/28 12:08
</commit_message>
<xml_diff>
--- a/res/SEED/res.xlsx
+++ b/res/SEED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78542E56-8AE4-B948-B270-E84745292A3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F648E1E0-26C2-7940-8181-E22130E29CCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -742,7 +742,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="4">
-        <v>0.9032</v>
+        <v>0.9133</v>
       </c>
       <c r="C22">
         <v>32</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="B32" s="7">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.93400333333333352</v>
+        <v>0.93434000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/05/31 6:53
</commit_message>
<xml_diff>
--- a/res/SEED/res.xlsx
+++ b/res/SEED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FBE8FA5-D03D-2148-8646-4E807888C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{870AF5CE-8A46-AD4A-9EF5-F41584F897F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -665,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="4">
-        <v>0.91259999999999997</v>
+        <v>0.92120000000000002</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="B32" s="7">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.93491666666666662</v>
+        <v>0.93520333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/05 16:08
</commit_message>
<xml_diff>
--- a/res/SEED/res.xlsx
+++ b/res/SEED/res.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/SEED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31259698-9C1E-714E-A8D2-3F7697CCF1C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22C8731-97F0-2143-AB32-815B22D8A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="141" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="141" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -665,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="4">
-        <v>0.92120000000000002</v>
+        <v>0.93569999999999998</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="B32" s="7">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.9353233333333334</v>
+        <v>0.9358066666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/07 23:50
</commit_message>
<xml_diff>
--- a/res/SEED/res.xlsx
+++ b/res/SEED/res.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22C8731-97F0-2143-AB32-815B22D8A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E0EEE-2785-2C45-9D0F-B43BEC400A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="141" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="141" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -665,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="4">
-        <v>0.93569999999999998</v>
+        <v>0.92120000000000002</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -786,7 +786,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="4">
-        <v>0.9032</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="C26">
         <v>37</v>
@@ -853,7 +853,7 @@
       </c>
       <c r="B32" s="7">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.9358066666666669</v>
+        <v>0.93595000000000017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new results. 2021/06/06 13:03
</commit_message>
<xml_diff>
--- a/res/SEED/res.xlsx
+++ b/res/SEED/res.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/PycharmProjects/Finegrained_GNN/res/SEED/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanyiik/Desktop/final_res/SEED/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E0EEE-2785-2C45-9D0F-B43BEC400A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBC1A6D-5129-9548-9D48-E46AAA354C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -188,10 +188,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="3" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="4" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="差" xfId="2" builtinId="27"/>
@@ -500,7 +500,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="141" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="200" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -665,7 +665,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="4">
-        <v>0.92120000000000002</v>
+        <v>0.93569999999999998</v>
       </c>
       <c r="C15">
         <v>20</v>
@@ -848,12 +848,12 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="6">
         <f>AVERAGE(B2:B31)</f>
-        <v>0.93595000000000017</v>
+        <v>0.93643333333333356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>